<commit_message>
fix resistor placement instead of caps, replace mic, fix count of components
</commit_message>
<xml_diff>
--- a/production/usbwledc-top-pos.xlsx
+++ b/production/usbwledc-top-pos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yannikmundler/Documents/GitHub/USBWLEDC/kicad/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yannikmundler/Documents/GitHub/USBWLEDC/production/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7AC207-895C-6146-AA61-C60C0E4B4FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC2321D-BDB6-974A-A579-76B9A5A17879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11680" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25680" yWindow="660" windowWidth="25380" windowHeight="28000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -142,12 +142,6 @@
     <t>MK1</t>
   </si>
   <si>
-    <t>GSA4737</t>
-  </si>
-  <si>
-    <t>Microphone-6pin</t>
-  </si>
-  <si>
     <t>Q1</t>
   </si>
   <si>
@@ -227,13 +221,19 @@
   </si>
   <si>
     <t>SOIC-16_3.9x9.9mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>ICS-43434</t>
+  </si>
+  <si>
+    <t>InvenSense_ICS-43434-6_3.5x2.65mm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,6 +247,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -292,7 +299,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -300,6 +307,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -584,7 +594,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -901,20 +911,20 @@
       <c r="A14" t="s">
         <v>32</v>
       </c>
-      <c r="B14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" t="s">
-        <v>34</v>
+      <c r="B14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="D14" s="2">
-        <v>30.531400000000001</v>
+        <v>32.6</v>
       </c>
       <c r="E14" s="2">
-        <v>-36.370800000000003</v>
+        <v>-38.299999999999997</v>
       </c>
       <c r="F14">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="G14" t="s">
         <v>11</v>
@@ -922,13 +932,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
         <v>35</v>
-      </c>
-      <c r="B15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" t="s">
-        <v>37</v>
       </c>
       <c r="D15" s="2">
         <v>44.1</v>
@@ -945,13 +955,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D16" s="2">
         <v>39.450000000000003</v>
@@ -968,13 +978,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
         <v>39</v>
-      </c>
-      <c r="B17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" t="s">
-        <v>41</v>
       </c>
       <c r="D17" s="2">
         <v>38.023800000000001</v>
@@ -994,10 +1004,10 @@
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D18" s="2">
         <v>38.023800000000001</v>
@@ -1014,13 +1024,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D19" s="2">
         <v>51.3</v>
@@ -1037,13 +1047,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
         <v>44</v>
-      </c>
-      <c r="B20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" t="s">
-        <v>46</v>
       </c>
       <c r="D20" s="2">
         <v>51.9938</v>
@@ -1060,13 +1070,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D21" s="2">
         <v>51.9938</v>
@@ -1083,13 +1093,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D22" s="2">
         <v>41.8</v>
@@ -1106,13 +1116,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D23" s="2">
         <v>41.8</v>
@@ -1129,13 +1139,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" t="s">
         <v>50</v>
-      </c>
-      <c r="B24" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" t="s">
-        <v>52</v>
       </c>
       <c r="D24" s="2">
         <v>45</v>
@@ -1152,13 +1162,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" t="s">
         <v>53</v>
-      </c>
-      <c r="B25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" t="s">
-        <v>55</v>
       </c>
       <c r="D25" s="2">
         <v>45</v>
@@ -1175,13 +1185,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" t="s">
         <v>56</v>
-      </c>
-      <c r="B26" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" t="s">
-        <v>58</v>
       </c>
       <c r="D26" s="2">
         <v>51.9</v>
@@ -1198,13 +1208,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" t="s">
         <v>59</v>
-      </c>
-      <c r="B27" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" t="s">
-        <v>61</v>
       </c>
       <c r="D27" s="2">
         <v>37.6</v>

</xml_diff>